<commit_message>
Update MTSOL_call and MTSET_call classes to enhance parameterization and increase iteration limits; add new validation files and update .gitignore for log files.
</commit_message>
<xml_diff>
--- a/Validation/X22 ducted propeller design.xlsx
+++ b/Validation/X22 ducted propeller design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b266c95a83fbf4bb/Documenten/TU Delft Aerospace Engineering/Msc2/AE5222 - Thesis/Software/Conceptual-Investigation-of-Alternative-Electric-Ducted-Fan-Architectures/Validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{BD216B15-C1D5-4986-A230-03396A0C0539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{310BFEDD-BB5A-4516-A261-6CD48C445E5F}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{BD216B15-C1D5-4986-A230-03396A0C0539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBC4C9C4-890B-416B-A238-0E8E970013DB}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{09A38DA9-5803-4F4A-AC50-1ACCD92E16A7}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{09A38DA9-5803-4F4A-AC50-1ACCD92E16A7}"/>
   </bookViews>
   <sheets>
     <sheet name="X22 geometry data" sheetId="1" r:id="rId1"/>
@@ -7485,15 +7485,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>55245</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>80010</xdr:rowOff>
+      <xdr:colOff>15660</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>169075</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>59055</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>108585</xdr:rowOff>
+      <xdr:colOff>19470</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>14572</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7922,7 +7922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97873B8E-A7D3-4C33-A17B-326DF912F514}">
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="90" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
@@ -10162,8 +10162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7245FA60-43DF-4342-887B-332FC6F471CF}">
   <dimension ref="A1:W78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O56" sqref="O56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -10224,7 +10224,7 @@
         <v>351.28199999999998</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I18" si="0">$E$4+(B2-$B$13)</f>
+        <f>$E$4+(B2-$B$13)</f>
         <v>38.699999999999996</v>
       </c>
       <c r="K2">
@@ -10261,15 +10261,15 @@
         <v>13</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G18" si="1">A3*0.5*$E$2*1000</f>
+        <f t="shared" ref="G3:G18" si="0">A3*0.5*$E$2*1000</f>
         <v>266.7</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H18" si="2">C3*1000</f>
+        <f t="shared" ref="H3:H18" si="1">C3*1000</f>
         <v>344.93200000000002</v>
       </c>
       <c r="I3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I3:I18" si="2">$E$4+(B3-$B$13)</f>
         <v>37.199999999999996</v>
       </c>
       <c r="K3">
@@ -10306,15 +10306,15 @@
         <v>19</v>
       </c>
       <c r="G4">
+        <f t="shared" si="0"/>
+        <v>320.03999999999996</v>
+      </c>
+      <c r="H4">
         <f t="shared" si="1"/>
-        <v>320.03999999999996</v>
-      </c>
-      <c r="H4">
+        <v>334.26400000000001</v>
+      </c>
+      <c r="I4">
         <f t="shared" si="2"/>
-        <v>334.26400000000001</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="0"/>
         <v>34.899999999999991</v>
       </c>
       <c r="K4">
@@ -10351,15 +10351,15 @@
         <v>17</v>
       </c>
       <c r="G5">
+        <f t="shared" si="0"/>
+        <v>373.38</v>
+      </c>
+      <c r="H5">
         <f t="shared" si="1"/>
-        <v>373.38</v>
-      </c>
-      <c r="H5">
+        <v>323.596</v>
+      </c>
+      <c r="I5">
         <f t="shared" si="2"/>
-        <v>323.596</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="0"/>
         <v>33.499999999999993</v>
       </c>
       <c r="K5">
@@ -10397,15 +10397,15 @@
         <v>1.2445999999999999</v>
       </c>
       <c r="G6">
+        <f t="shared" si="0"/>
+        <v>426.71999999999997</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="1"/>
-        <v>426.71999999999997</v>
-      </c>
-      <c r="H6">
+        <v>314.19800000000004</v>
+      </c>
+      <c r="I6">
         <f t="shared" si="2"/>
-        <v>314.19800000000004</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
         <v>31.6</v>
       </c>
       <c r="K6">
@@ -10439,15 +10439,15 @@
         <v>0.24079999999999999</v>
       </c>
       <c r="G7">
+        <f t="shared" si="0"/>
+        <v>480.06</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="1"/>
-        <v>480.06</v>
-      </c>
-      <c r="H7">
+        <v>305.81599999999997</v>
+      </c>
+      <c r="I7">
         <f t="shared" si="2"/>
-        <v>305.81599999999997</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="0"/>
         <v>29.899999999999991</v>
       </c>
       <c r="K7">
@@ -10484,15 +10484,15 @@
         <v>18</v>
       </c>
       <c r="G8">
+        <f t="shared" si="0"/>
+        <v>533.4</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="1"/>
-        <v>533.4</v>
-      </c>
-      <c r="H8">
+        <v>296.92599999999999</v>
+      </c>
+      <c r="I8">
         <f t="shared" si="2"/>
-        <v>296.92599999999999</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
         <v>27.999999999999993</v>
       </c>
       <c r="K8">
@@ -10530,15 +10530,15 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="G9">
+        <f t="shared" si="0"/>
+        <v>586.74</v>
+      </c>
+      <c r="H9">
         <f t="shared" si="1"/>
-        <v>586.74</v>
-      </c>
-      <c r="H9">
+        <v>288.54399999999998</v>
+      </c>
+      <c r="I9">
         <f t="shared" si="2"/>
-        <v>288.54399999999998</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="0"/>
         <v>26.199999999999996</v>
       </c>
       <c r="K9">
@@ -10572,15 +10572,15 @@
         <v>0.20879999999999999</v>
       </c>
       <c r="G10">
+        <f t="shared" si="0"/>
+        <v>640.07999999999993</v>
+      </c>
+      <c r="H10">
         <f t="shared" si="1"/>
-        <v>640.07999999999993</v>
-      </c>
-      <c r="H10">
+        <v>279.654</v>
+      </c>
+      <c r="I10">
         <f t="shared" si="2"/>
-        <v>279.654</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
         <v>24.299999999999997</v>
       </c>
       <c r="K10">
@@ -10617,15 +10617,15 @@
         <v>24</v>
       </c>
       <c r="G11">
+        <f t="shared" si="0"/>
+        <v>693.42000000000007</v>
+      </c>
+      <c r="H11">
         <f t="shared" si="1"/>
-        <v>693.42000000000007</v>
-      </c>
-      <c r="H11">
+        <v>270.25599999999997</v>
+      </c>
+      <c r="I11">
         <f t="shared" si="2"/>
-        <v>270.25599999999997</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="0"/>
         <v>22.499999999999993</v>
       </c>
       <c r="K11">
@@ -10663,15 +10663,15 @@
         <v>0.35560000000000003</v>
       </c>
       <c r="G12">
+        <f t="shared" si="0"/>
+        <v>746.76</v>
+      </c>
+      <c r="H12">
         <f t="shared" si="1"/>
-        <v>746.76</v>
-      </c>
-      <c r="H12">
+        <v>263.14400000000001</v>
+      </c>
+      <c r="I12">
         <f t="shared" si="2"/>
-        <v>263.14400000000001</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="0"/>
         <v>20.599999999999994</v>
       </c>
       <c r="K12">
@@ -10705,15 +10705,15 @@
         <v>0.1832</v>
       </c>
       <c r="G13">
+        <f t="shared" si="0"/>
+        <v>800.1</v>
+      </c>
+      <c r="H13">
         <f t="shared" si="1"/>
-        <v>800.1</v>
-      </c>
-      <c r="H13">
+        <v>256.79399999999998</v>
+      </c>
+      <c r="I13">
         <f t="shared" si="2"/>
-        <v>256.79399999999998</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="K13">
@@ -10747,15 +10747,15 @@
         <v>0.17519999999999999</v>
       </c>
       <c r="G14">
+        <f t="shared" si="0"/>
+        <v>853.43999999999994</v>
+      </c>
+      <c r="H14">
         <f t="shared" si="1"/>
-        <v>853.43999999999994</v>
-      </c>
-      <c r="H14">
+        <v>253.23800000000003</v>
+      </c>
+      <c r="I14">
         <f t="shared" si="2"/>
-        <v>253.23800000000003</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="0"/>
         <v>17.199999999999996</v>
       </c>
       <c r="K14">
@@ -10789,15 +10789,15 @@
         <v>0.16760000000000003</v>
       </c>
       <c r="G15">
+        <f t="shared" si="0"/>
+        <v>906.78</v>
+      </c>
+      <c r="H15">
         <f t="shared" si="1"/>
-        <v>906.78</v>
-      </c>
-      <c r="H15">
+        <v>248.66599999999997</v>
+      </c>
+      <c r="I15">
         <f t="shared" si="2"/>
-        <v>248.66599999999997</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="0"/>
         <v>15.499999999999996</v>
       </c>
       <c r="K15">
@@ -10831,15 +10831,15 @@
         <v>0.16079999999999997</v>
       </c>
       <c r="G16">
+        <f t="shared" si="0"/>
+        <v>960.12</v>
+      </c>
+      <c r="H16">
         <f t="shared" si="1"/>
-        <v>960.12</v>
-      </c>
-      <c r="H16">
+        <v>245.87199999999999</v>
+      </c>
+      <c r="I16">
         <f t="shared" si="2"/>
-        <v>245.87199999999999</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="0"/>
         <v>13.699999999999996</v>
       </c>
       <c r="K16">
@@ -10873,15 +10873,15 @@
         <v>0.15279999999999999</v>
       </c>
       <c r="G17">
+        <f t="shared" si="0"/>
+        <v>1013.46</v>
+      </c>
+      <c r="H17">
         <f t="shared" si="1"/>
-        <v>1013.46</v>
-      </c>
-      <c r="H17">
+        <v>243.33200000000002</v>
+      </c>
+      <c r="I17">
         <f t="shared" si="2"/>
-        <v>243.33200000000002</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="0"/>
         <v>12.599999999999994</v>
       </c>
       <c r="K17">
@@ -10915,15 +10915,15 @@
         <v>0.14599999999999999</v>
       </c>
       <c r="G18">
+        <f t="shared" si="0"/>
+        <v>1066.8</v>
+      </c>
+      <c r="H18">
         <f t="shared" si="1"/>
-        <v>1066.8</v>
-      </c>
-      <c r="H18">
+        <v>241.80799999999996</v>
+      </c>
+      <c r="I18">
         <f t="shared" si="2"/>
-        <v>241.80799999999996</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="0"/>
         <v>11.199999999999996</v>
       </c>
       <c r="K18">

</xml_diff>

<commit_message>
Add new validation data files for X22A and update existing validation datasets
</commit_message>
<xml_diff>
--- a/Validation/X22 ducted propeller design.xlsx
+++ b/Validation/X22 ducted propeller design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b266c95a83fbf4bb/Documenten/TU Delft Aerospace Engineering/Msc2/AE5222 - Thesis/Software/Conceptual-Investigation-of-Alternative-Electric-Ducted-Fan-Architectures/Validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{BD216B15-C1D5-4986-A230-03396A0C0539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBC4C9C4-890B-416B-A238-0E8E970013DB}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{BD216B15-C1D5-4986-A230-03396A0C0539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72CF5A2B-6CF6-4EA5-B35C-E0D1636B11A7}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{09A38DA9-5803-4F4A-AC50-1ACCD92E16A7}"/>
   </bookViews>
@@ -7603,6 +7603,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7922,8 +7926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97873B8E-A7D3-4C33-A17B-326DF912F514}">
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="90" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="C15" zoomScale="90" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AE33" sqref="AE33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -9306,7 +9310,7 @@
         <v>27.9</v>
       </c>
       <c r="C58">
-        <f t="shared" si="1"/>
+        <f>(E17+8)*2.54/100</f>
         <v>0.24333200000000002</v>
       </c>
       <c r="D58">

</xml_diff>

<commit_message>
seems to be running. results are closer, but not quite there yet.
</commit_message>
<xml_diff>
--- a/Validation/X22 ducted propeller design.xlsx
+++ b/Validation/X22 ducted propeller design.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b266c95a83fbf4bb/Documenten/TU Delft Aerospace Engineering/Msc2/AE5222 - Thesis/Software/Conceptual-Investigation-of-Alternative-Electric-Ducted-Fan-Architectures/Validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{BD216B15-C1D5-4986-A230-03396A0C0539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72CF5A2B-6CF6-4EA5-B35C-E0D1636B11A7}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{BD216B15-C1D5-4986-A230-03396A0C0539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4764A625-4B80-4504-9C22-26A3E963562D}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{09A38DA9-5803-4F4A-AC50-1ACCD92E16A7}"/>
+    <workbookView xWindow="12525" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{09A38DA9-5803-4F4A-AC50-1ACCD92E16A7}"/>
   </bookViews>
   <sheets>
     <sheet name="X22 geometry data" sheetId="1" r:id="rId1"/>
@@ -7926,7 +7926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97873B8E-A7D3-4C33-A17B-326DF912F514}">
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" zoomScale="90" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="C15" zoomScale="90" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AE33" sqref="AE33"/>
     </sheetView>
   </sheetViews>
@@ -10166,8 +10166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7245FA60-43DF-4342-887B-332FC6F471CF}">
   <dimension ref="A1:W78"/>
   <sheetViews>
-    <sheetView zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O56" sqref="O56"/>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -10229,7 +10229,7 @@
       </c>
       <c r="I2">
         <f>$E$4+(B2-$B$13)</f>
-        <v>38.699999999999996</v>
+        <v>48.699999999999996</v>
       </c>
       <c r="K2">
         <f>G2/1000</f>
@@ -10241,7 +10241,7 @@
       </c>
       <c r="M2">
         <f>I2</f>
-        <v>38.699999999999996</v>
+        <v>48.699999999999996</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -10274,7 +10274,7 @@
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I18" si="2">$E$4+(B3-$B$13)</f>
-        <v>37.199999999999996</v>
+        <v>47.199999999999996</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K18" si="3">G3/1000</f>
@@ -10286,7 +10286,7 @@
       </c>
       <c r="M3">
         <f t="shared" ref="M3:M18" si="5">I3</f>
-        <v>37.199999999999996</v>
+        <v>47.199999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -10307,7 +10307,7 @@
         <v>0.28439999999999999</v>
       </c>
       <c r="E4">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
@@ -10319,7 +10319,7 @@
       </c>
       <c r="I4">
         <f t="shared" si="2"/>
-        <v>34.899999999999991</v>
+        <v>44.899999999999991</v>
       </c>
       <c r="K4">
         <f t="shared" si="3"/>
@@ -10331,7 +10331,7 @@
       </c>
       <c r="M4">
         <f t="shared" si="5"/>
-        <v>34.899999999999991</v>
+        <v>44.899999999999991</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -10364,7 +10364,7 @@
       </c>
       <c r="I5">
         <f t="shared" si="2"/>
-        <v>33.499999999999993</v>
+        <v>43.499999999999993</v>
       </c>
       <c r="K5">
         <f t="shared" si="3"/>
@@ -10376,7 +10376,7 @@
       </c>
       <c r="M5">
         <f t="shared" si="5"/>
-        <v>33.499999999999993</v>
+        <v>43.499999999999993</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -10410,7 +10410,7 @@
       </c>
       <c r="I6">
         <f t="shared" si="2"/>
-        <v>31.6</v>
+        <v>41.6</v>
       </c>
       <c r="K6">
         <f t="shared" si="3"/>
@@ -10422,7 +10422,7 @@
       </c>
       <c r="M6">
         <f t="shared" si="5"/>
-        <v>31.6</v>
+        <v>41.6</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -10452,7 +10452,7 @@
       </c>
       <c r="I7">
         <f t="shared" si="2"/>
-        <v>29.899999999999991</v>
+        <v>39.899999999999991</v>
       </c>
       <c r="K7">
         <f t="shared" si="3"/>
@@ -10464,7 +10464,7 @@
       </c>
       <c r="M7">
         <f t="shared" si="5"/>
-        <v>29.899999999999991</v>
+        <v>39.899999999999991</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -10497,7 +10497,7 @@
       </c>
       <c r="I8">
         <f t="shared" si="2"/>
-        <v>27.999999999999993</v>
+        <v>37.999999999999993</v>
       </c>
       <c r="K8">
         <f t="shared" si="3"/>
@@ -10509,7 +10509,7 @@
       </c>
       <c r="M8">
         <f t="shared" si="5"/>
-        <v>27.999999999999993</v>
+        <v>37.999999999999993</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -10543,7 +10543,7 @@
       </c>
       <c r="I9">
         <f t="shared" si="2"/>
-        <v>26.199999999999996</v>
+        <v>36.199999999999996</v>
       </c>
       <c r="K9">
         <f t="shared" si="3"/>
@@ -10555,7 +10555,7 @@
       </c>
       <c r="M9">
         <f t="shared" si="5"/>
-        <v>26.199999999999996</v>
+        <v>36.199999999999996</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -10585,7 +10585,7 @@
       </c>
       <c r="I10">
         <f t="shared" si="2"/>
-        <v>24.299999999999997</v>
+        <v>34.299999999999997</v>
       </c>
       <c r="K10">
         <f t="shared" si="3"/>
@@ -10597,7 +10597,7 @@
       </c>
       <c r="M10">
         <f t="shared" si="5"/>
-        <v>24.299999999999997</v>
+        <v>34.299999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -10630,7 +10630,7 @@
       </c>
       <c r="I11">
         <f t="shared" si="2"/>
-        <v>22.499999999999993</v>
+        <v>32.499999999999993</v>
       </c>
       <c r="K11">
         <f t="shared" si="3"/>
@@ -10642,7 +10642,7 @@
       </c>
       <c r="M11">
         <f t="shared" si="5"/>
-        <v>22.499999999999993</v>
+        <v>32.499999999999993</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -10676,7 +10676,7 @@
       </c>
       <c r="I12">
         <f t="shared" si="2"/>
-        <v>20.599999999999994</v>
+        <v>30.599999999999994</v>
       </c>
       <c r="K12">
         <f t="shared" si="3"/>
@@ -10688,7 +10688,7 @@
       </c>
       <c r="M12">
         <f t="shared" si="5"/>
-        <v>20.599999999999994</v>
+        <v>30.599999999999994</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -10718,7 +10718,7 @@
       </c>
       <c r="I13">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="K13">
         <f t="shared" si="3"/>
@@ -10730,7 +10730,7 @@
       </c>
       <c r="M13">
         <f t="shared" si="5"/>
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -10760,7 +10760,7 @@
       </c>
       <c r="I14">
         <f t="shared" si="2"/>
-        <v>17.199999999999996</v>
+        <v>27.199999999999996</v>
       </c>
       <c r="K14">
         <f t="shared" si="3"/>
@@ -10772,7 +10772,7 @@
       </c>
       <c r="M14">
         <f t="shared" si="5"/>
-        <v>17.199999999999996</v>
+        <v>27.199999999999996</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -10802,7 +10802,7 @@
       </c>
       <c r="I15">
         <f t="shared" si="2"/>
-        <v>15.499999999999996</v>
+        <v>25.499999999999996</v>
       </c>
       <c r="K15">
         <f t="shared" si="3"/>
@@ -10814,7 +10814,7 @@
       </c>
       <c r="M15">
         <f t="shared" si="5"/>
-        <v>15.499999999999996</v>
+        <v>25.499999999999996</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -10844,7 +10844,7 @@
       </c>
       <c r="I16">
         <f t="shared" si="2"/>
-        <v>13.699999999999996</v>
+        <v>23.699999999999996</v>
       </c>
       <c r="K16">
         <f t="shared" si="3"/>
@@ -10856,7 +10856,7 @@
       </c>
       <c r="M16">
         <f t="shared" si="5"/>
-        <v>13.699999999999996</v>
+        <v>23.699999999999996</v>
       </c>
     </row>
     <row r="17" spans="1:23">
@@ -10886,7 +10886,7 @@
       </c>
       <c r="I17">
         <f t="shared" si="2"/>
-        <v>12.599999999999994</v>
+        <v>22.599999999999994</v>
       </c>
       <c r="K17">
         <f t="shared" si="3"/>
@@ -10898,7 +10898,7 @@
       </c>
       <c r="M17">
         <f t="shared" si="5"/>
-        <v>12.599999999999994</v>
+        <v>22.599999999999994</v>
       </c>
     </row>
     <row r="18" spans="1:23">
@@ -10928,7 +10928,7 @@
       </c>
       <c r="I18">
         <f t="shared" si="2"/>
-        <v>11.199999999999996</v>
+        <v>21.199999999999996</v>
       </c>
       <c r="K18">
         <f t="shared" si="3"/>
@@ -10940,7 +10940,7 @@
       </c>
       <c r="M18">
         <f t="shared" si="5"/>
-        <v>11.199999999999996</v>
+        <v>21.199999999999996</v>
       </c>
     </row>
     <row r="21" spans="1:23">

</xml_diff>

<commit_message>
Seems to be working! Slight issue at lower values of J when running the loop....
</commit_message>
<xml_diff>
--- a/Validation/X22 ducted propeller design.xlsx
+++ b/Validation/X22 ducted propeller design.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{BD216B15-C1D5-4986-A230-03396A0C0539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4764A625-4B80-4504-9C22-26A3E963562D}"/>
   <bookViews>
-    <workbookView xWindow="12525" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{09A38DA9-5803-4F4A-AC50-1ACCD92E16A7}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{09A38DA9-5803-4F4A-AC50-1ACCD92E16A7}"/>
   </bookViews>
   <sheets>
     <sheet name="X22 geometry data" sheetId="1" r:id="rId1"/>
@@ -7603,10 +7603,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -10166,8 +10162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7245FA60-43DF-4342-887B-332FC6F471CF}">
   <dimension ref="A1:W78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22:R36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Following a discussion with professor Sinnige, the next step will be to pause validation on the X22A, and instead use the TUD XPROP. This removes a duct, and, given the more detailed results, should make validation of the input routines easier
</commit_message>
<xml_diff>
--- a/Validation/X22 ducted propeller design.xlsx
+++ b/Validation/X22 ducted propeller design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b266c95a83fbf4bb/Documenten/TU Delft Aerospace Engineering/Msc2/AE5222 - Thesis/Software/Conceptual-Investigation-of-Alternative-Electric-Ducted-Fan-Architectures/Validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{BD216B15-C1D5-4986-A230-03396A0C0539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4764A625-4B80-4504-9C22-26A3E963562D}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{BD216B15-C1D5-4986-A230-03396A0C0539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DB28AB6-94B5-4173-A46A-517C08651D89}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{09A38DA9-5803-4F4A-AC50-1ACCD92E16A7}"/>
+    <workbookView xWindow="39160" yWindow="760" windowWidth="28800" windowHeight="15290" activeTab="2" xr2:uid="{09A38DA9-5803-4F4A-AC50-1ACCD92E16A7}"/>
   </bookViews>
   <sheets>
     <sheet name="X22 geometry data" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>r/R</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>sweep_angle</t>
   </si>
 </sst>
 </file>
@@ -7603,6 +7606,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7922,11 +7929,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97873B8E-A7D3-4C33-A17B-326DF912F514}">
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView topLeftCell="C15" zoomScale="90" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AE33" sqref="AE33"/>
+    <sheetView zoomScale="90" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
@@ -9483,9 +9490,9 @@
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.7890625" style="2"/>
+    <col min="1" max="1" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -10162,13 +10169,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7245FA60-43DF-4342-887B-332FC6F471CF}">
   <dimension ref="A1:W78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22:R36"/>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10193,8 +10200,11 @@
       <c r="I1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="Q1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2">
         <f>'X22 geometry data'!A43</f>
         <v>0.2</v>
@@ -10239,8 +10249,15 @@
         <f>I2</f>
         <v>48.699999999999996</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="O2">
+        <v>0.41909999999999997</v>
+      </c>
+      <c r="Q2">
+        <f>DEGREES(ATAN(($O$2-C2)/(2*A2*1.0647)))</f>
+        <v>9.047928016483775</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3">
         <f>'X22 geometry data'!A44</f>
         <v>0.25</v>
@@ -10284,8 +10301,12 @@
         <f t="shared" ref="M3:M18" si="5">I3</f>
         <v>47.199999999999996</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q18" si="6">DEGREES(ATAN(($O$2-C3)/(2*A3*1.0647)))</f>
+        <v>7.9315000278308654</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4">
         <f>'X22 geometry data'!A45</f>
         <v>0.3</v>
@@ -10329,8 +10350,12 @@
         <f t="shared" si="5"/>
         <v>44.899999999999991</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="Q4">
+        <f t="shared" si="6"/>
+        <v>7.5646793316892493</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5">
         <f>'X22 geometry data'!A46</f>
         <v>0.35</v>
@@ -10374,8 +10399,12 @@
         <f t="shared" si="5"/>
         <v>43.499999999999993</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="Q5">
+        <f t="shared" si="6"/>
+        <v>7.3022803422810876</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6">
         <f>'X22 geometry data'!A47</f>
         <v>0.4</v>
@@ -10420,8 +10449,12 @@
         <f t="shared" si="5"/>
         <v>41.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="Q6">
+        <f t="shared" si="6"/>
+        <v>7.0211401615147171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7">
         <f>'X22 geometry data'!A48</f>
         <v>0.45</v>
@@ -10462,8 +10495,12 @@
         <f t="shared" si="5"/>
         <v>39.899999999999991</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="Q7">
+        <f t="shared" si="6"/>
+        <v>6.742334462821189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8">
         <f>'X22 geometry data'!A49</f>
         <v>0.5</v>
@@ -10507,8 +10544,12 @@
         <f t="shared" si="5"/>
         <v>37.999999999999993</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="Q8">
+        <f t="shared" si="6"/>
+        <v>6.5460417541860902</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9">
         <f>'X22 geometry data'!A50</f>
         <v>0.55000000000000004</v>
@@ -10553,8 +10594,12 @@
         <f t="shared" si="5"/>
         <v>36.199999999999996</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="Q9">
+        <f t="shared" si="6"/>
+        <v>6.3607774678505624</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10">
         <f>'X22 geometry data'!A51</f>
         <v>0.6</v>
@@ -10595,8 +10640,12 @@
         <f t="shared" si="5"/>
         <v>34.299999999999997</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="Q10">
+        <f t="shared" si="6"/>
+        <v>6.2288023553099494</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11">
         <f>'X22 geometry data'!A52</f>
         <v>0.65</v>
@@ -10640,8 +10689,12 @@
         <f t="shared" si="5"/>
         <v>32.499999999999993</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="Q11">
+        <f t="shared" si="6"/>
+        <v>6.137868462238683</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12">
         <f>'X22 geometry data'!A53</f>
         <v>0.7</v>
@@ -10686,8 +10739,12 @@
         <f t="shared" si="5"/>
         <v>30.599999999999994</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="Q12">
+        <f t="shared" si="6"/>
+        <v>5.9729951601249303</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13">
         <f>'X22 geometry data'!A54</f>
         <v>0.75</v>
@@ -10728,8 +10785,12 @@
         <f t="shared" si="5"/>
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="Q13">
+        <f t="shared" si="6"/>
+        <v>5.8029677643258912</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14">
         <f>'X22 geometry data'!A55</f>
         <v>0.8</v>
@@ -10770,8 +10831,12 @@
         <f t="shared" si="5"/>
         <v>27.199999999999996</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="Q14">
+        <f t="shared" si="6"/>
+        <v>5.5610340778763385</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15">
         <f>'X22 geometry data'!A56</f>
         <v>0.85</v>
@@ -10812,8 +10877,12 @@
         <f t="shared" si="5"/>
         <v>25.499999999999996</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="Q15">
+        <f t="shared" si="6"/>
+        <v>5.3792783604436867</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16">
         <f>'X22 geometry data'!A57</f>
         <v>0.9</v>
@@ -10853,6 +10922,10 @@
       <c r="M16">
         <f t="shared" si="5"/>
         <v>23.699999999999996</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="6"/>
+        <v>5.1649052971725746</v>
       </c>
     </row>
     <row r="17" spans="1:23">
@@ -10896,6 +10969,10 @@
         <f t="shared" si="5"/>
         <v>22.599999999999994</v>
       </c>
+      <c r="Q17">
+        <f t="shared" si="6"/>
+        <v>4.9658345526352052</v>
+      </c>
     </row>
     <row r="18" spans="1:23">
       <c r="A18">
@@ -10938,6 +11015,10 @@
         <f t="shared" si="5"/>
         <v>21.199999999999996</v>
       </c>
+      <c r="Q18">
+        <f t="shared" si="6"/>
+        <v>4.7594196771492276</v>
+      </c>
     </row>
     <row r="21" spans="1:23">
       <c r="B21" t="s">
@@ -10959,7 +11040,7 @@
         <v>45.326599999999999</v>
       </c>
       <c r="E22">
-        <f t="shared" ref="E22:E53" si="6">A22*2.54/100</f>
+        <f t="shared" ref="E22:E53" si="7">A22*2.54/100</f>
         <v>1.23952</v>
       </c>
       <c r="F22">
@@ -10990,11 +11071,11 @@
         <v>5</v>
       </c>
       <c r="S22">
-        <f t="shared" ref="S22:S52" si="7">(Q22-3.4)*2.54/100</f>
+        <f t="shared" ref="S22:S52" si="8">(Q22-3.4)*2.54/100</f>
         <v>1.0820400000000001</v>
       </c>
       <c r="T22">
-        <f t="shared" ref="T22:T36" si="8">R22*2.54/100</f>
+        <f t="shared" ref="T22:T36" si="9">R22*2.54/100</f>
         <v>0.127</v>
       </c>
       <c r="U22">
@@ -11017,23 +11098,23 @@
         <v>42.7</v>
       </c>
       <c r="C23">
-        <f t="shared" ref="C23:C78" si="9">(B23-47.625)*0.416+47.625</f>
+        <f t="shared" ref="C23:C78" si="10">(B23-47.625)*0.416+47.625</f>
         <v>45.5762</v>
       </c>
       <c r="E23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.2166600000000001</v>
       </c>
       <c r="F23">
-        <f t="shared" ref="F23:F78" si="10">C23*2.54/100</f>
+        <f t="shared" ref="F23:F78" si="11">C23*2.54/100</f>
         <v>1.1576354799999999</v>
       </c>
       <c r="G23">
-        <f t="shared" ref="G23:G77" si="11">E23*1000</f>
+        <f t="shared" ref="G23:G77" si="12">E23*1000</f>
         <v>1216.6600000000001</v>
       </c>
       <c r="H23">
-        <f t="shared" ref="H23:H78" si="12">F23*1000</f>
+        <f t="shared" ref="H23:H78" si="13">F23*1000</f>
         <v>1157.6354799999999</v>
       </c>
       <c r="I23">
@@ -11049,19 +11130,19 @@
         <v>5.2</v>
       </c>
       <c r="S23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.05664</v>
       </c>
       <c r="T23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.13208</v>
       </c>
       <c r="U23">
-        <f t="shared" ref="U23:U52" si="13">S23*1000</f>
+        <f t="shared" ref="U23:U52" si="14">S23*1000</f>
         <v>1056.6400000000001</v>
       </c>
       <c r="V23">
-        <f t="shared" ref="V23:V52" si="14">T23*1000</f>
+        <f t="shared" ref="V23:V52" si="15">T23*1000</f>
         <v>132.08000000000001</v>
       </c>
       <c r="W23">
@@ -11076,23 +11157,23 @@
         <v>44</v>
       </c>
       <c r="C24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>46.116999999999997</v>
       </c>
       <c r="E24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.143</v>
       </c>
       <c r="F24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.1713718</v>
       </c>
       <c r="G24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1143</v>
       </c>
       <c r="H24">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1171.3717999999999</v>
       </c>
       <c r="I24">
@@ -11105,19 +11186,19 @@
         <v>5.6</v>
       </c>
       <c r="S24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.0058400000000001</v>
       </c>
       <c r="T24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.14223999999999998</v>
       </c>
       <c r="U24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1005.84</v>
       </c>
       <c r="V24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>142.23999999999998</v>
       </c>
       <c r="W24">
@@ -11132,23 +11213,23 @@
         <v>45.4</v>
       </c>
       <c r="C25">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>46.699399999999997</v>
       </c>
       <c r="E25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.05664</v>
       </c>
       <c r="F25">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.1861647599999998</v>
       </c>
       <c r="G25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1056.6400000000001</v>
       </c>
       <c r="H25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1186.1647599999999</v>
       </c>
       <c r="I25">
@@ -11161,19 +11242,19 @@
         <v>6.2</v>
       </c>
       <c r="S25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.92964000000000002</v>
       </c>
       <c r="T25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.15748000000000001</v>
       </c>
       <c r="U25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>929.64</v>
       </c>
       <c r="V25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>157.48000000000002</v>
       </c>
       <c r="W25">
@@ -11188,23 +11269,23 @@
         <v>46.8</v>
       </c>
       <c r="C26">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>47.281799999999997</v>
       </c>
       <c r="E26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.96774000000000004</v>
       </c>
       <c r="F26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.2009577199999999</v>
       </c>
       <c r="G26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>967.74</v>
       </c>
       <c r="H26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1200.9577199999999</v>
       </c>
       <c r="I26">
@@ -11217,19 +11298,19 @@
         <v>7.1</v>
       </c>
       <c r="S26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.77724000000000004</v>
       </c>
       <c r="T26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.18034</v>
       </c>
       <c r="U26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>777.24</v>
       </c>
       <c r="V26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>180.34</v>
       </c>
       <c r="W26">
@@ -11244,23 +11325,23 @@
         <v>47.6</v>
       </c>
       <c r="C27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>47.614600000000003</v>
       </c>
       <c r="E27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.91948000000000008</v>
       </c>
       <c r="F27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.2094108400000001</v>
       </c>
       <c r="G27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>919.48</v>
       </c>
       <c r="H27">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1209.41084</v>
       </c>
       <c r="I27">
@@ -11273,19 +11354,19 @@
         <v>7.8</v>
       </c>
       <c r="S27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.72644000000000009</v>
       </c>
       <c r="T27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.19812000000000002</v>
       </c>
       <c r="U27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>726.44</v>
       </c>
       <c r="V27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>198.12</v>
       </c>
       <c r="W27">
@@ -11300,23 +11381,23 @@
         <v>48.9</v>
       </c>
       <c r="C28">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>48.1554</v>
       </c>
       <c r="E28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.83311999999999997</v>
       </c>
       <c r="F28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.2231471600000001</v>
       </c>
       <c r="G28">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>833.12</v>
       </c>
       <c r="H28">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1223.1471600000002</v>
       </c>
       <c r="I28">
@@ -11329,19 +11410,19 @@
         <v>8.5</v>
       </c>
       <c r="S28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.67564000000000002</v>
       </c>
       <c r="T28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.21590000000000001</v>
       </c>
       <c r="U28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>675.64</v>
       </c>
       <c r="V28">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>215.9</v>
       </c>
       <c r="W28">
@@ -11356,23 +11437,23 @@
         <v>50.2</v>
       </c>
       <c r="C29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>48.696200000000005</v>
       </c>
       <c r="E29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.74167999999999989</v>
       </c>
       <c r="F29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.2368834800000001</v>
       </c>
       <c r="G29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>741.68</v>
       </c>
       <c r="H29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1236.8834800000002</v>
       </c>
       <c r="I29">
@@ -11385,19 +11466,19 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="S29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.54864000000000002</v>
       </c>
       <c r="T29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.22097999999999998</v>
       </c>
       <c r="U29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>548.64</v>
       </c>
       <c r="V29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>220.98</v>
       </c>
       <c r="W29">
@@ -11412,23 +11493,23 @@
         <v>51.2</v>
       </c>
       <c r="C30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>49.112200000000001</v>
       </c>
       <c r="E30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.66294000000000008</v>
       </c>
       <c r="F30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.24744988</v>
       </c>
       <c r="G30">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>662.94</v>
       </c>
       <c r="H30">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1247.4498800000001</v>
       </c>
       <c r="I30">
@@ -11441,19 +11522,19 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="S30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.47244000000000008</v>
       </c>
       <c r="T30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.20827999999999999</v>
       </c>
       <c r="U30">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>472.44000000000005</v>
       </c>
       <c r="V30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>208.28</v>
       </c>
       <c r="W30">
@@ -11468,23 +11549,23 @@
         <v>51.9</v>
       </c>
       <c r="C31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>49.403399999999998</v>
       </c>
       <c r="E31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.59182000000000001</v>
       </c>
       <c r="F31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.2548463599999999</v>
       </c>
       <c r="G31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>591.82000000000005</v>
       </c>
       <c r="H31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1254.84636</v>
       </c>
       <c r="I31">
@@ -11497,19 +11578,19 @@
         <v>7.5</v>
       </c>
       <c r="S31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.39624000000000004</v>
       </c>
       <c r="T31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.1905</v>
       </c>
       <c r="U31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>396.24</v>
       </c>
       <c r="V31">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>190.5</v>
       </c>
       <c r="W31">
@@ -11524,23 +11605,23 @@
         <v>52.4</v>
       </c>
       <c r="C32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>49.611399999999996</v>
       </c>
       <c r="E32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.52070000000000005</v>
       </c>
       <c r="F32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.26012956</v>
       </c>
       <c r="G32">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>520.70000000000005</v>
       </c>
       <c r="H32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1260.1295600000001</v>
       </c>
       <c r="I32">
@@ -11553,19 +11634,19 @@
         <v>6.5</v>
       </c>
       <c r="S32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.29464000000000001</v>
       </c>
       <c r="T32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.16510000000000002</v>
       </c>
       <c r="U32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>294.64</v>
       </c>
       <c r="V32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>165.10000000000002</v>
       </c>
       <c r="W32">
@@ -11580,23 +11661,23 @@
         <v>52.6</v>
       </c>
       <c r="C33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>49.694600000000001</v>
       </c>
       <c r="E33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.44195999999999996</v>
       </c>
       <c r="F33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.2622428400000001</v>
       </c>
       <c r="G33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>441.96</v>
       </c>
       <c r="H33">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1262.2428400000001</v>
       </c>
       <c r="I33">
@@ -11609,19 +11690,19 @@
         <v>5.6</v>
       </c>
       <c r="S33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.19303999999999999</v>
       </c>
       <c r="T33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.14223999999999998</v>
       </c>
       <c r="U33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>193.04</v>
       </c>
       <c r="V33">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>142.23999999999998</v>
       </c>
       <c r="W33">
@@ -11636,23 +11717,23 @@
         <v>53</v>
       </c>
       <c r="C34">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>49.860999999999997</v>
       </c>
       <c r="E34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.36829999999999996</v>
       </c>
       <c r="F34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.2664694000000001</v>
       </c>
       <c r="G34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>368.29999999999995</v>
       </c>
       <c r="H34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1266.4694000000002</v>
       </c>
       <c r="I34">
@@ -11665,19 +11746,19 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="S34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.3660000000000003E-2</v>
       </c>
       <c r="T34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.11176000000000003</v>
       </c>
       <c r="U34">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>73.66</v>
       </c>
       <c r="V34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>111.76000000000002</v>
       </c>
       <c r="W34">
@@ -11692,23 +11773,23 @@
         <v>53</v>
       </c>
       <c r="C35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>49.860999999999997</v>
       </c>
       <c r="E35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.27940000000000004</v>
       </c>
       <c r="F35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.2664694000000001</v>
       </c>
       <c r="G35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>279.40000000000003</v>
       </c>
       <c r="H35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1266.4694000000002</v>
       </c>
       <c r="I35">
@@ -11721,19 +11802,19 @@
         <v>3.3</v>
       </c>
       <c r="S35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-2.7940000000000006E-2</v>
       </c>
       <c r="T35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8.3819999999999992E-2</v>
       </c>
       <c r="U35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-27.940000000000005</v>
       </c>
       <c r="V35">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>83.82</v>
       </c>
       <c r="W35">
@@ -11748,23 +11829,23 @@
         <v>53</v>
       </c>
       <c r="C36">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>49.860999999999997</v>
       </c>
       <c r="E36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.2286</v>
       </c>
       <c r="F36">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.2664694000000001</v>
       </c>
       <c r="G36">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>228.6</v>
       </c>
       <c r="H36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1266.4694000000002</v>
       </c>
       <c r="I36">
@@ -11777,19 +11858,19 @@
         <v>1.7</v>
       </c>
       <c r="S36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-8.6359999999999992E-2</v>
       </c>
       <c r="T36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4.3179999999999996E-2</v>
       </c>
       <c r="U36">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-86.359999999999985</v>
       </c>
       <c r="V36">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>43.179999999999993</v>
       </c>
       <c r="W36">
@@ -11804,23 +11885,23 @@
         <v>52.8</v>
       </c>
       <c r="C37">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>49.777799999999999</v>
       </c>
       <c r="E37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.15798799999999999</v>
       </c>
       <c r="F37">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.26435612</v>
       </c>
       <c r="G37">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>157.988</v>
       </c>
       <c r="H37">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1264.3561199999999</v>
       </c>
       <c r="I37">
@@ -11837,15 +11918,15 @@
         <v>-8.6359999999999992E-2</v>
       </c>
       <c r="T37">
-        <f t="shared" ref="T37:T52" si="15">R37*2.54/100</f>
+        <f t="shared" ref="T37:T52" si="16">R37*2.54/100</f>
         <v>0</v>
       </c>
       <c r="U37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-86.359999999999985</v>
       </c>
       <c r="V37">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="W37">
@@ -11860,23 +11941,23 @@
         <v>52.5</v>
       </c>
       <c r="C38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>49.652999999999999</v>
       </c>
       <c r="E38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.120396</v>
       </c>
       <c r="F38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.2611862</v>
       </c>
       <c r="G38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>120.396</v>
       </c>
       <c r="H38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1261.1862000000001</v>
       </c>
       <c r="I38">
@@ -11889,19 +11970,19 @@
         <v>-1.7</v>
       </c>
       <c r="S38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-8.6359999999999992E-2</v>
       </c>
       <c r="T38">
+        <f t="shared" si="16"/>
+        <v>-4.3179999999999996E-2</v>
+      </c>
+      <c r="U38">
+        <f t="shared" si="14"/>
+        <v>-86.359999999999985</v>
+      </c>
+      <c r="V38">
         <f t="shared" si="15"/>
-        <v>-4.3179999999999996E-2</v>
-      </c>
-      <c r="U38">
-        <f t="shared" si="13"/>
-        <v>-86.359999999999985</v>
-      </c>
-      <c r="V38">
-        <f t="shared" si="14"/>
         <v>-43.179999999999993</v>
       </c>
       <c r="W38">
@@ -11916,23 +11997,23 @@
         <v>52.3</v>
       </c>
       <c r="C39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>49.569800000000001</v>
       </c>
       <c r="E39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.7536000000000012E-2</v>
       </c>
       <c r="F39">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.2590729199999999</v>
       </c>
       <c r="G39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>97.536000000000016</v>
       </c>
       <c r="H39">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1259.0729199999998</v>
       </c>
       <c r="I39">
@@ -11945,19 +12026,19 @@
         <v>-3.3</v>
       </c>
       <c r="S39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-2.7940000000000006E-2</v>
       </c>
       <c r="T39">
+        <f t="shared" si="16"/>
+        <v>-8.3819999999999992E-2</v>
+      </c>
+      <c r="U39">
+        <f t="shared" si="14"/>
+        <v>-27.940000000000005</v>
+      </c>
+      <c r="V39">
         <f t="shared" si="15"/>
-        <v>-8.3819999999999992E-2</v>
-      </c>
-      <c r="U39">
-        <f t="shared" si="13"/>
-        <v>-27.940000000000005</v>
-      </c>
-      <c r="V39">
-        <f t="shared" si="14"/>
         <v>-83.82</v>
       </c>
       <c r="W39">
@@ -11972,23 +12053,23 @@
         <v>52</v>
       </c>
       <c r="C40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>49.445</v>
       </c>
       <c r="E40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.8740000000000004E-2</v>
       </c>
       <c r="F40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.255903</v>
       </c>
       <c r="G40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>78.740000000000009</v>
       </c>
       <c r="H40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1255.903</v>
       </c>
       <c r="I40">
@@ -12007,19 +12088,19 @@
         <v>-4.4000000000000004</v>
       </c>
       <c r="S40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.3660000000000003E-2</v>
       </c>
       <c r="T40">
+        <f t="shared" si="16"/>
+        <v>-0.11176000000000003</v>
+      </c>
+      <c r="U40">
+        <f t="shared" si="14"/>
+        <v>73.66</v>
+      </c>
+      <c r="V40">
         <f t="shared" si="15"/>
-        <v>-0.11176000000000003</v>
-      </c>
-      <c r="U40">
-        <f t="shared" si="13"/>
-        <v>73.66</v>
-      </c>
-      <c r="V40">
-        <f t="shared" si="14"/>
         <v>-111.76000000000002</v>
       </c>
       <c r="W40">
@@ -12034,23 +12115,23 @@
         <v>51.4</v>
       </c>
       <c r="C41">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>49.195399999999999</v>
       </c>
       <c r="E41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.7911999999999998E-2</v>
       </c>
       <c r="F41">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.2495631600000001</v>
       </c>
       <c r="G41">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>57.911999999999999</v>
       </c>
       <c r="H41">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1249.5631600000002</v>
       </c>
       <c r="I41">
@@ -12069,19 +12150,19 @@
         <v>-5.6</v>
       </c>
       <c r="S41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.19303999999999999</v>
       </c>
       <c r="T41">
+        <f t="shared" si="16"/>
+        <v>-0.14223999999999998</v>
+      </c>
+      <c r="U41">
+        <f t="shared" si="14"/>
+        <v>193.04</v>
+      </c>
+      <c r="V41">
         <f t="shared" si="15"/>
-        <v>-0.14223999999999998</v>
-      </c>
-      <c r="U41">
-        <f t="shared" si="13"/>
-        <v>193.04</v>
-      </c>
-      <c r="V41">
-        <f t="shared" si="14"/>
         <v>-142.23999999999998</v>
       </c>
       <c r="W41">
@@ -12096,23 +12177,23 @@
         <v>50.9</v>
       </c>
       <c r="C42">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>48.987400000000001</v>
       </c>
       <c r="E42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.1148000000000004E-2</v>
       </c>
       <c r="F42">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.2442799600000001</v>
       </c>
       <c r="G42">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>41.148000000000003</v>
       </c>
       <c r="H42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1244.2799600000001</v>
       </c>
       <c r="I42">
@@ -12131,19 +12212,19 @@
         <v>-6.5</v>
       </c>
       <c r="S42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.29464000000000001</v>
       </c>
       <c r="T42">
+        <f t="shared" si="16"/>
+        <v>-0.16510000000000002</v>
+      </c>
+      <c r="U42">
+        <f t="shared" si="14"/>
+        <v>294.64</v>
+      </c>
+      <c r="V42">
         <f t="shared" si="15"/>
-        <v>-0.16510000000000002</v>
-      </c>
-      <c r="U42">
-        <f t="shared" si="13"/>
-        <v>294.64</v>
-      </c>
-      <c r="V42">
-        <f t="shared" si="14"/>
         <v>-165.10000000000002</v>
       </c>
       <c r="W42">
@@ -12158,23 +12239,23 @@
         <v>50.5</v>
       </c>
       <c r="C43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>48.820999999999998</v>
       </c>
       <c r="E43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.9718000000000001E-2</v>
       </c>
       <c r="F43">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.2400533999999999</v>
       </c>
       <c r="G43">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>29.718</v>
       </c>
       <c r="H43">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1240.0533999999998</v>
       </c>
       <c r="I43">
@@ -12193,19 +12274,19 @@
         <v>-7.5</v>
       </c>
       <c r="S43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.39624000000000004</v>
       </c>
       <c r="T43">
+        <f t="shared" si="16"/>
+        <v>-0.1905</v>
+      </c>
+      <c r="U43">
+        <f t="shared" si="14"/>
+        <v>396.24</v>
+      </c>
+      <c r="V43">
         <f t="shared" si="15"/>
-        <v>-0.1905</v>
-      </c>
-      <c r="U43">
-        <f t="shared" si="13"/>
-        <v>396.24</v>
-      </c>
-      <c r="V43">
-        <f t="shared" si="14"/>
         <v>-190.5</v>
       </c>
       <c r="W43">
@@ -12220,23 +12301,23 @@
         <v>49.9</v>
       </c>
       <c r="C44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>48.571399999999997</v>
       </c>
       <c r="E44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.0447000000000003E-2</v>
       </c>
       <c r="F44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.23371356</v>
       </c>
       <c r="G44">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>20.447000000000003</v>
       </c>
       <c r="H44">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1233.7135599999999</v>
       </c>
       <c r="I44">
@@ -12255,19 +12336,19 @@
         <v>-8.1999999999999993</v>
       </c>
       <c r="S44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.47244000000000008</v>
       </c>
       <c r="T44">
+        <f t="shared" si="16"/>
+        <v>-0.20827999999999999</v>
+      </c>
+      <c r="U44">
+        <f t="shared" si="14"/>
+        <v>472.44000000000005</v>
+      </c>
+      <c r="V44">
         <f t="shared" si="15"/>
-        <v>-0.20827999999999999</v>
-      </c>
-      <c r="U44">
-        <f t="shared" si="13"/>
-        <v>472.44000000000005</v>
-      </c>
-      <c r="V44">
-        <f t="shared" si="14"/>
         <v>-208.28</v>
       </c>
       <c r="W44">
@@ -12282,23 +12363,23 @@
         <v>49.1</v>
       </c>
       <c r="C45">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>48.238599999999998</v>
       </c>
       <c r="E45">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.10998E-2</v>
       </c>
       <c r="F45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.22526044</v>
       </c>
       <c r="G45">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11.0998</v>
       </c>
       <c r="H45">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1225.26044</v>
       </c>
       <c r="I45">
@@ -12317,19 +12398,19 @@
         <v>-8.6999999999999993</v>
       </c>
       <c r="S45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.54864000000000002</v>
       </c>
       <c r="T45">
+        <f t="shared" si="16"/>
+        <v>-0.22097999999999998</v>
+      </c>
+      <c r="U45">
+        <f t="shared" si="14"/>
+        <v>548.64</v>
+      </c>
+      <c r="V45">
         <f t="shared" si="15"/>
-        <v>-0.22097999999999998</v>
-      </c>
-      <c r="U45">
-        <f t="shared" si="13"/>
-        <v>548.64</v>
-      </c>
-      <c r="V45">
-        <f t="shared" si="14"/>
         <v>-220.98</v>
       </c>
       <c r="W45">
@@ -12344,23 +12425,23 @@
         <v>48.1</v>
       </c>
       <c r="C46">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>47.822600000000001</v>
       </c>
       <c r="E46">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.7084000000000002E-3</v>
       </c>
       <c r="F46">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.2146940400000001</v>
       </c>
       <c r="G46">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3.7084000000000001</v>
       </c>
       <c r="H46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1214.6940400000001</v>
       </c>
       <c r="I46">
@@ -12379,19 +12460,19 @@
         <v>-8.5</v>
       </c>
       <c r="S46">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.67564000000000002</v>
       </c>
       <c r="T46">
+        <f t="shared" si="16"/>
+        <v>-0.21590000000000001</v>
+      </c>
+      <c r="U46">
+        <f t="shared" si="14"/>
+        <v>675.64</v>
+      </c>
+      <c r="V46">
         <f t="shared" si="15"/>
-        <v>-0.21590000000000001</v>
-      </c>
-      <c r="U46">
-        <f t="shared" si="13"/>
-        <v>675.64</v>
-      </c>
-      <c r="V46">
-        <f t="shared" si="14"/>
         <v>-215.9</v>
       </c>
       <c r="W46">
@@ -12406,23 +12487,23 @@
         <v>46.7</v>
       </c>
       <c r="C47">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>47.240200000000002</v>
       </c>
       <c r="E47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F47">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.1999010800000001</v>
       </c>
       <c r="G47">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="H47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1199.9010800000001</v>
       </c>
       <c r="I47">
@@ -12441,19 +12522,19 @@
         <v>-7.8</v>
       </c>
       <c r="S47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.72644000000000009</v>
       </c>
       <c r="T47">
+        <f t="shared" si="16"/>
+        <v>-0.19812000000000002</v>
+      </c>
+      <c r="U47">
+        <f t="shared" si="14"/>
+        <v>726.44</v>
+      </c>
+      <c r="V47">
         <f t="shared" si="15"/>
-        <v>-0.19812000000000002</v>
-      </c>
-      <c r="U47">
-        <f t="shared" si="13"/>
-        <v>726.44</v>
-      </c>
-      <c r="V47">
-        <f t="shared" si="14"/>
         <v>-198.12</v>
       </c>
       <c r="W47">
@@ -12468,23 +12549,23 @@
         <v>45.5</v>
       </c>
       <c r="C48">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>46.741</v>
       </c>
       <c r="E48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.5400000000000005E-4</v>
       </c>
       <c r="F48">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.1872213999999999</v>
       </c>
       <c r="G48">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.25400000000000006</v>
       </c>
       <c r="H48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1187.2213999999999</v>
       </c>
       <c r="I48">
@@ -12503,19 +12584,19 @@
         <v>-7.1</v>
       </c>
       <c r="S48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.77724000000000004</v>
       </c>
       <c r="T48">
+        <f t="shared" si="16"/>
+        <v>-0.18034</v>
+      </c>
+      <c r="U48">
+        <f t="shared" si="14"/>
+        <v>777.24</v>
+      </c>
+      <c r="V48">
         <f t="shared" si="15"/>
-        <v>-0.18034</v>
-      </c>
-      <c r="U48">
-        <f t="shared" si="13"/>
-        <v>777.24</v>
-      </c>
-      <c r="V48">
-        <f t="shared" si="14"/>
         <v>-180.34</v>
       </c>
       <c r="W48">
@@ -12530,23 +12611,23 @@
         <v>44.2</v>
       </c>
       <c r="C49">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>46.200200000000002</v>
       </c>
       <c r="E49">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.4358599999999998E-3</v>
       </c>
       <c r="F49">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.1734850800000001</v>
       </c>
       <c r="G49">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.4358599999999999</v>
       </c>
       <c r="H49">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1173.4850800000002</v>
       </c>
       <c r="I49">
@@ -12565,19 +12646,19 @@
         <v>-6.2</v>
       </c>
       <c r="S49">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.92964000000000002</v>
       </c>
       <c r="T49">
+        <f t="shared" si="16"/>
+        <v>-0.15748000000000001</v>
+      </c>
+      <c r="U49">
+        <f t="shared" si="14"/>
+        <v>929.64</v>
+      </c>
+      <c r="V49">
         <f t="shared" si="15"/>
-        <v>-0.15748000000000001</v>
-      </c>
-      <c r="U49">
-        <f t="shared" si="13"/>
-        <v>929.64</v>
-      </c>
-      <c r="V49">
-        <f t="shared" si="14"/>
         <v>-157.48000000000002</v>
       </c>
       <c r="W49">
@@ -12592,23 +12673,23 @@
         <v>43.2</v>
       </c>
       <c r="C50">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>45.784199999999998</v>
       </c>
       <c r="E50">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8.2804000000000003E-3</v>
       </c>
       <c r="F50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.16291868</v>
       </c>
       <c r="G50">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>8.2804000000000002</v>
       </c>
       <c r="H50">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1162.91868</v>
       </c>
       <c r="I50">
@@ -12627,19 +12708,19 @@
         <v>-5.6</v>
       </c>
       <c r="S50">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.0058400000000001</v>
       </c>
       <c r="T50">
+        <f t="shared" si="16"/>
+        <v>-0.14223999999999998</v>
+      </c>
+      <c r="U50">
+        <f t="shared" si="14"/>
+        <v>1005.84</v>
+      </c>
+      <c r="V50">
         <f t="shared" si="15"/>
-        <v>-0.14223999999999998</v>
-      </c>
-      <c r="U50">
-        <f t="shared" si="13"/>
-        <v>1005.84</v>
-      </c>
-      <c r="V50">
-        <f t="shared" si="14"/>
         <v>-142.23999999999998</v>
       </c>
       <c r="W50">
@@ -12654,23 +12735,23 @@
         <v>41.7</v>
       </c>
       <c r="C51">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>45.160200000000003</v>
       </c>
       <c r="E51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.7957799999999999E-2</v>
       </c>
       <c r="F51">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.1470690800000001</v>
       </c>
       <c r="G51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>17.957799999999999</v>
       </c>
       <c r="H51">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1147.06908</v>
       </c>
       <c r="I51">
@@ -12689,19 +12770,19 @@
         <v>-5.2</v>
       </c>
       <c r="S51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.05664</v>
       </c>
       <c r="T51">
+        <f t="shared" si="16"/>
+        <v>-0.13208</v>
+      </c>
+      <c r="U51">
+        <f t="shared" si="14"/>
+        <v>1056.6400000000001</v>
+      </c>
+      <c r="V51">
         <f t="shared" si="15"/>
-        <v>-0.13208</v>
-      </c>
-      <c r="U51">
-        <f t="shared" si="13"/>
-        <v>1056.6400000000001</v>
-      </c>
-      <c r="V51">
-        <f t="shared" si="14"/>
         <v>-132.08000000000001</v>
       </c>
       <c r="W51">
@@ -12716,23 +12797,23 @@
         <v>40.299999999999997</v>
       </c>
       <c r="C52">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>44.577799999999996</v>
       </c>
       <c r="E52">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.3274000000000005E-2</v>
       </c>
       <c r="F52">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.13227612</v>
       </c>
       <c r="G52">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>33.274000000000008</v>
       </c>
       <c r="H52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1132.27612</v>
       </c>
       <c r="I52">
@@ -12751,19 +12832,19 @@
         <v>-5</v>
       </c>
       <c r="S52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.0820400000000001</v>
       </c>
       <c r="T52">
+        <f t="shared" si="16"/>
+        <v>-0.127</v>
+      </c>
+      <c r="U52">
+        <f t="shared" si="14"/>
+        <v>1082.0400000000002</v>
+      </c>
+      <c r="V52">
         <f t="shared" si="15"/>
-        <v>-0.127</v>
-      </c>
-      <c r="U52">
-        <f t="shared" si="13"/>
-        <v>1082.0400000000002</v>
-      </c>
-      <c r="V52">
-        <f t="shared" si="14"/>
         <v>-127</v>
       </c>
       <c r="W52">
@@ -12778,23 +12859,23 @@
         <v>38.700000000000003</v>
       </c>
       <c r="C53">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>43.912199999999999</v>
       </c>
       <c r="E53">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.6388000000000008E-2</v>
       </c>
       <c r="F53">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.11536988</v>
       </c>
       <c r="G53">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>56.388000000000005</v>
       </c>
       <c r="H53">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1115.36988</v>
       </c>
       <c r="I53">
@@ -12815,23 +12896,23 @@
         <v>37.4</v>
       </c>
       <c r="C54">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>43.371400000000001</v>
       </c>
       <c r="E54">
-        <f t="shared" ref="E54:E77" si="16">A54*2.54/100</f>
+        <f t="shared" ref="E54:E77" si="17">A54*2.54/100</f>
         <v>8.6868000000000001E-2</v>
       </c>
       <c r="F54">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.10163356</v>
       </c>
       <c r="G54">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>86.867999999999995</v>
       </c>
       <c r="H54">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1101.63356</v>
       </c>
       <c r="I54">
@@ -12852,23 +12933,23 @@
         <v>36.4</v>
       </c>
       <c r="C55">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>42.955399999999997</v>
       </c>
       <c r="E55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.11531600000000002</v>
       </c>
       <c r="F55">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.0910671599999999</v>
       </c>
       <c r="G55">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>115.31600000000002</v>
       </c>
       <c r="H55">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1091.0671599999998</v>
       </c>
       <c r="I55">
@@ -12889,23 +12970,23 @@
         <v>35.799999999999997</v>
       </c>
       <c r="C56">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>42.705799999999996</v>
       </c>
       <c r="E56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.14757399999999998</v>
       </c>
       <c r="F56">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.0847273199999998</v>
       </c>
       <c r="G56">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>147.57399999999998</v>
       </c>
       <c r="H56">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1084.7273199999997</v>
       </c>
       <c r="I56">
@@ -12926,23 +13007,23 @@
         <v>35.4</v>
       </c>
       <c r="C57">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>42.539400000000001</v>
       </c>
       <c r="E57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.183642</v>
       </c>
       <c r="F57">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.0805007600000001</v>
       </c>
       <c r="G57">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>183.642</v>
       </c>
       <c r="H57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1080.5007600000001</v>
       </c>
       <c r="I57">
@@ -12963,23 +13044,23 @@
         <v>35.1</v>
       </c>
       <c r="C58">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>42.4146</v>
       </c>
       <c r="E58">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.21767800000000001</v>
       </c>
       <c r="F58">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.0773308400000001</v>
       </c>
       <c r="G58">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>217.678</v>
       </c>
       <c r="H58">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1077.3308400000001</v>
       </c>
       <c r="I58">
@@ -13000,23 +13081,23 @@
         <v>35.1</v>
       </c>
       <c r="C59">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>42.4146</v>
       </c>
       <c r="E59">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.253492</v>
       </c>
       <c r="F59">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.0773308400000001</v>
       </c>
       <c r="G59">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>253.49199999999999</v>
       </c>
       <c r="H59">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1077.3308400000001</v>
       </c>
       <c r="I59">
@@ -13041,19 +13122,19 @@
         <v>42.372999999999998</v>
       </c>
       <c r="E60">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.30226000000000003</v>
       </c>
       <c r="F60">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.0762742000000001</v>
       </c>
       <c r="G60">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>302.26000000000005</v>
       </c>
       <c r="H60">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1076.2742000000001</v>
       </c>
       <c r="I60">
@@ -13074,23 +13155,23 @@
         <v>35</v>
       </c>
       <c r="C61">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>42.372999999999998</v>
       </c>
       <c r="E61">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.34543999999999997</v>
       </c>
       <c r="F61">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.0762742000000001</v>
       </c>
       <c r="G61">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>345.43999999999994</v>
       </c>
       <c r="H61">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1076.2742000000001</v>
       </c>
       <c r="I61">
@@ -13105,23 +13186,23 @@
         <v>35</v>
       </c>
       <c r="C62">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>42.372999999999998</v>
       </c>
       <c r="E62">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.40132000000000007</v>
       </c>
       <c r="F62">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.0762742000000001</v>
       </c>
       <c r="G62">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>401.32000000000005</v>
       </c>
       <c r="H62">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1076.2742000000001</v>
       </c>
       <c r="I62">
@@ -13136,23 +13217,23 @@
         <v>35</v>
       </c>
       <c r="C63">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>42.372999999999998</v>
       </c>
       <c r="E63">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.46482000000000001</v>
       </c>
       <c r="F63">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.0762742000000001</v>
       </c>
       <c r="G63">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>464.82</v>
       </c>
       <c r="H63">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1076.2742000000001</v>
       </c>
       <c r="I63">
@@ -13167,23 +13248,23 @@
         <v>35.200000000000003</v>
       </c>
       <c r="C64">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>42.456200000000003</v>
       </c>
       <c r="E64">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.54355999999999993</v>
       </c>
       <c r="F64">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.0783874800000002</v>
       </c>
       <c r="G64">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>543.55999999999995</v>
       </c>
       <c r="H64">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1078.3874800000001</v>
       </c>
       <c r="I64">
@@ -13198,23 +13279,23 @@
         <v>35.6</v>
       </c>
       <c r="C65">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>42.622599999999998</v>
       </c>
       <c r="E65">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.61468</v>
       </c>
       <c r="F65">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.0826140399999999</v>
       </c>
       <c r="G65">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>614.67999999999995</v>
       </c>
       <c r="H65">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1082.6140399999999</v>
       </c>
       <c r="I65">
@@ -13229,23 +13310,23 @@
         <v>36.1</v>
       </c>
       <c r="C66">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>42.830600000000004</v>
       </c>
       <c r="E66">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.71120000000000005</v>
       </c>
       <c r="F66">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.08789724</v>
       </c>
       <c r="G66">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>711.2</v>
       </c>
       <c r="H66">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1087.89724</v>
       </c>
       <c r="I66">
@@ -13260,23 +13341,23 @@
         <v>36.799999999999997</v>
       </c>
       <c r="C67">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>43.1218</v>
       </c>
       <c r="E67">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.78993999999999998</v>
       </c>
       <c r="F67">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.0952937200000001</v>
       </c>
       <c r="G67">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>789.93999999999994</v>
       </c>
       <c r="H67">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1095.2937200000001</v>
       </c>
       <c r="I67">
@@ -13291,23 +13372,23 @@
         <v>37.299999999999997</v>
       </c>
       <c r="C68">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>43.329799999999999</v>
       </c>
       <c r="E68">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.84836</v>
       </c>
       <c r="F68">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.10057692</v>
       </c>
       <c r="G68">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>848.36</v>
       </c>
       <c r="H68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1100.57692</v>
       </c>
       <c r="I68">
@@ -13322,23 +13403,23 @@
         <v>37.799999999999997</v>
       </c>
       <c r="C69">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>43.537799999999997</v>
       </c>
       <c r="E69">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.91185999999999989</v>
       </c>
       <c r="F69">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.10586012</v>
       </c>
       <c r="G69">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>911.8599999999999</v>
       </c>
       <c r="H69">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1105.8601200000001</v>
       </c>
       <c r="I69">
@@ -13353,23 +13434,23 @@
         <v>38.4</v>
       </c>
       <c r="C70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>43.787399999999998</v>
       </c>
       <c r="E70">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.96519999999999995</v>
       </c>
       <c r="F70">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.1121999599999999</v>
       </c>
       <c r="G70">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>965.19999999999993</v>
       </c>
       <c r="H70">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1112.1999599999999</v>
       </c>
       <c r="I70">
@@ -13384,23 +13465,23 @@
         <v>38.9</v>
       </c>
       <c r="C71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>43.995399999999997</v>
       </c>
       <c r="E71">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.0058400000000001</v>
       </c>
       <c r="F71">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.1174831599999999</v>
       </c>
       <c r="G71">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1005.84</v>
       </c>
       <c r="H71">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1117.48316</v>
       </c>
       <c r="I71">
@@ -13415,23 +13496,23 @@
         <v>39.299999999999997</v>
       </c>
       <c r="C72">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>44.161799999999999</v>
       </c>
       <c r="E72">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.05918</v>
       </c>
       <c r="F72">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.1217097200000001</v>
       </c>
       <c r="G72">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1059.18</v>
       </c>
       <c r="H72">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1121.7097200000001</v>
       </c>
       <c r="I72">
@@ -13446,23 +13527,23 @@
         <v>40.1</v>
       </c>
       <c r="C73">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>44.494599999999998</v>
       </c>
       <c r="E73">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.1150599999999999</v>
       </c>
       <c r="F73">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.1301628399999999</v>
       </c>
       <c r="G73">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1115.06</v>
       </c>
       <c r="H73">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1130.16284</v>
       </c>
       <c r="I73">
@@ -13477,23 +13558,23 @@
         <v>40.5</v>
       </c>
       <c r="C74">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>44.661000000000001</v>
       </c>
       <c r="E74">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.1557000000000002</v>
       </c>
       <c r="F74">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.1343894000000001</v>
       </c>
       <c r="G74">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1155.7000000000003</v>
       </c>
       <c r="H74">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1134.3894</v>
       </c>
       <c r="I74">
@@ -13508,23 +13589,23 @@
         <v>41</v>
       </c>
       <c r="C75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>44.869</v>
       </c>
       <c r="E75">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.1988799999999999</v>
       </c>
       <c r="F75">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.1396725999999999</v>
       </c>
       <c r="G75">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1198.8799999999999</v>
       </c>
       <c r="H75">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1139.6725999999999</v>
       </c>
       <c r="I75">
@@ -13539,23 +13620,23 @@
         <v>41.3</v>
       </c>
       <c r="C76">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>44.9938</v>
       </c>
       <c r="E76">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.22936</v>
       </c>
       <c r="F76">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.1428425200000001</v>
       </c>
       <c r="G76">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1229.3599999999999</v>
       </c>
       <c r="H76">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1142.8425200000001</v>
       </c>
       <c r="I76">
@@ -13570,23 +13651,23 @@
         <v>41.6</v>
       </c>
       <c r="C77">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>45.118600000000001</v>
       </c>
       <c r="E77">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.23952</v>
       </c>
       <c r="F77">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.14601244</v>
       </c>
       <c r="G77">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1239.52</v>
       </c>
       <c r="H77">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1146.01244</v>
       </c>
       <c r="I77">
@@ -13598,15 +13679,15 @@
         <v>0</v>
       </c>
       <c r="C78">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>27.813000000000002</v>
       </c>
       <c r="F78">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.70645020000000003</v>
       </c>
       <c r="H78">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>706.4502</v>
       </c>
     </row>
@@ -13625,7 +13706,7 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
@@ -14139,7 +14220,7 @@
       <selection activeCell="E2" sqref="E2:G92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -16259,7 +16340,7 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1">

</xml_diff>

<commit_message>
updated constraints, repair, main files, and utils. Fixed issue with LE point positioning in file_handling.
</commit_message>
<xml_diff>
--- a/Validation/X22 ducted propeller design.xlsx
+++ b/Validation/X22 ducted propeller design.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b266c95a83fbf4bb/Documenten/TU Delft Aerospace Engineering/Msc2/AE5222 - Thesis/Software/Conceptual-Investigation-of-Alternative-Electric-Ducted-Fan-Architectures/Validation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\OneDrive\Documenten\TU Delft Aerospace Engineering\Msc2\AE5222 - Thesis\Software\Conceptual-Investigation-of-Alternative-Electric-Ducted-Fan-Architectures\Validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{BD216B15-C1D5-4986-A230-03396A0C0539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DB28AB6-94B5-4173-A46A-517C08651D89}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85ED6776-C4D8-4E62-AB2A-AD3DD39C3C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39160" yWindow="760" windowWidth="28800" windowHeight="15290" activeTab="2" xr2:uid="{09A38DA9-5803-4F4A-AC50-1ACCD92E16A7}"/>
+    <workbookView xWindow="4330" yWindow="3340" windowWidth="28800" windowHeight="15200" activeTab="2" xr2:uid="{09A38DA9-5803-4F4A-AC50-1ACCD92E16A7}"/>
   </bookViews>
   <sheets>
     <sheet name="X22 geometry data" sheetId="1" r:id="rId1"/>
-    <sheet name="Airfoil (NACA0018)" sheetId="6" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Performance" sheetId="4" r:id="rId4"/>
-    <sheet name="Airfoil (NACA 2408)" sheetId="3" r:id="rId5"/>
-    <sheet name="Airfoil (NACA 2410)" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Performance" sheetId="4" r:id="rId3"/>
+    <sheet name="Airfoil (NACA 2408)" sheetId="3" r:id="rId4"/>
+    <sheet name="Airfoil (NACA 2410)" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -149,7 +148,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,12 +159,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial Unicode MS"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -188,12 +181,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7606,10 +7598,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7930,7 +7918,7 @@
   <dimension ref="A1:K68"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -9483,694 +9471,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60FBDE77-DFE5-4714-9E0C-ED7A061E72A0}">
-  <dimension ref="A1:F35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="8.81640625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>1.89E-3</v>
-      </c>
-      <c r="D1">
-        <f>A1*1000</f>
-        <v>1000</v>
-      </c>
-      <c r="E1">
-        <f>B1*1000</f>
-        <v>1.89</v>
-      </c>
-      <c r="F1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="B2">
-        <v>1.21E-2</v>
-      </c>
-      <c r="D2">
-        <f t="shared" ref="D2:D35" si="0">A2*1000</f>
-        <v>950</v>
-      </c>
-      <c r="E2">
-        <f t="shared" ref="E2:E35" si="1">B2*1000</f>
-        <v>12.1</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="B3">
-        <v>2.172E-2</v>
-      </c>
-      <c r="D3">
-        <f t="shared" si="0"/>
-        <v>900</v>
-      </c>
-      <c r="E3">
-        <f t="shared" si="1"/>
-        <v>21.72</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="B4">
-        <v>3.9350000000000003E-2</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>800</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="1"/>
-        <v>39.35</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="B5">
-        <v>5.4960000000000002E-2</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>700</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="1"/>
-        <v>54.96</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="B6">
-        <v>6.8449999999999997E-2</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>600</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="1"/>
-        <v>68.45</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="B7">
-        <v>7.9409999999999994E-2</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="1"/>
-        <v>79.41</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="B8">
-        <v>8.7050000000000002E-2</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>400</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="1"/>
-        <v>87.05</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="B9">
-        <v>9.0029999999999999E-2</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>300</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="1"/>
-        <v>90.03</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="B10">
-        <v>8.9120000000000005E-2</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>250</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="1"/>
-        <v>89.12</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="B11">
-        <v>8.6059999999999998E-2</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="1"/>
-        <v>86.06</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="B12">
-        <v>8.0180000000000001E-2</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="1"/>
-        <v>80.180000000000007</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="B13">
-        <v>7.0239999999999997E-2</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="1"/>
-        <v>70.239999999999995</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="1">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="B14">
-        <v>6.3E-2</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="1"/>
-        <v>63</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="B15">
-        <v>5.3319999999999999E-2</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="1"/>
-        <v>53.32</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="1">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="B16">
-        <v>3.9219999999999998E-2</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="1"/>
-        <v>39.22</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="1">
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="B17">
-        <v>2.8410000000000001E-2</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>12.5</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="1"/>
-        <v>28.41</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="1">
-        <v>0</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="1">
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="B19">
-        <v>-2.8410000000000001E-2</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>12.5</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="1"/>
-        <v>-28.41</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="1">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="B20">
-        <v>-3.9219999999999998E-2</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="1"/>
-        <v>-39.22</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="B21">
-        <v>-5.3319999999999999E-2</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="1"/>
-        <v>-53.32</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="1">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="B22">
-        <v>-6.3E-2</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="1"/>
-        <v>-63</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="B23">
-        <v>-7.0239999999999997E-2</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="1"/>
-        <v>-70.239999999999995</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="B24">
-        <v>-8.0180000000000001E-2</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="1"/>
-        <v>-80.180000000000007</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="B25">
-        <v>-8.6059999999999998E-2</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="1"/>
-        <v>-86.06</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="B26">
-        <v>-8.9120000000000005E-2</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="0"/>
-        <v>250</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="1"/>
-        <v>-89.12</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="B27">
-        <v>-9.0029999999999999E-2</v>
-      </c>
-      <c r="D27">
-        <f t="shared" si="0"/>
-        <v>300</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="1"/>
-        <v>-90.03</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="B28">
-        <v>-8.7050000000000002E-2</v>
-      </c>
-      <c r="D28">
-        <f t="shared" si="0"/>
-        <v>400</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="1"/>
-        <v>-87.05</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="B29">
-        <v>-7.9409999999999994E-2</v>
-      </c>
-      <c r="D29">
-        <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-      <c r="E29">
-        <f t="shared" si="1"/>
-        <v>-79.41</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="B30">
-        <v>-6.8449999999999997E-2</v>
-      </c>
-      <c r="D30">
-        <f t="shared" si="0"/>
-        <v>600</v>
-      </c>
-      <c r="E30">
-        <f t="shared" si="1"/>
-        <v>-68.45</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="B31">
-        <v>-5.4960000000000002E-2</v>
-      </c>
-      <c r="D31">
-        <f t="shared" si="0"/>
-        <v>700</v>
-      </c>
-      <c r="E31">
-        <f t="shared" si="1"/>
-        <v>-54.96</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="B32">
-        <v>-3.9350000000000003E-2</v>
-      </c>
-      <c r="D32">
-        <f t="shared" si="0"/>
-        <v>800</v>
-      </c>
-      <c r="E32">
-        <f t="shared" si="1"/>
-        <v>-39.35</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="B33">
-        <v>-2.172E-2</v>
-      </c>
-      <c r="D33">
-        <f t="shared" si="0"/>
-        <v>900</v>
-      </c>
-      <c r="E33">
-        <f t="shared" si="1"/>
-        <v>-21.72</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="B34">
-        <v>-1.21E-2</v>
-      </c>
-      <c r="D34">
-        <f t="shared" si="0"/>
-        <v>950</v>
-      </c>
-      <c r="E34">
-        <f t="shared" si="1"/>
-        <v>-12.1</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="1">
-        <v>1</v>
-      </c>
-      <c r="B35">
-        <v>-1.89E-3</v>
-      </c>
-      <c r="D35">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="E35">
-        <f t="shared" si="1"/>
-        <v>-1.89</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7245FA60-43DF-4342-887B-332FC6F471CF}">
   <dimension ref="A1:W78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -10210,8 +9515,7 @@
         <v>0.2</v>
       </c>
       <c r="B2">
-        <f>'X22 geometry data'!B43</f>
-        <v>54</v>
+        <v>53.6</v>
       </c>
       <c r="C2">
         <f>'X22 geometry data'!C43</f>
@@ -10235,7 +9539,7 @@
       </c>
       <c r="I2">
         <f>$E$4+(B2-$B$13)</f>
-        <v>48.699999999999996</v>
+        <v>52.6</v>
       </c>
       <c r="K2">
         <f>G2/1000</f>
@@ -10247,7 +9551,7 @@
       </c>
       <c r="M2">
         <f>I2</f>
-        <v>48.699999999999996</v>
+        <v>52.6</v>
       </c>
       <c r="O2">
         <v>0.41909999999999997</v>
@@ -10263,8 +9567,7 @@
         <v>0.25</v>
       </c>
       <c r="B3">
-        <f>'X22 geometry data'!B44</f>
-        <v>52.5</v>
+        <v>50</v>
       </c>
       <c r="C3">
         <f>'X22 geometry data'!C44</f>
@@ -10287,7 +9590,7 @@
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I18" si="2">$E$4+(B3-$B$13)</f>
-        <v>47.199999999999996</v>
+        <v>49</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K18" si="3">G3/1000</f>
@@ -10299,7 +9602,7 @@
       </c>
       <c r="M3">
         <f t="shared" ref="M3:M18" si="5">I3</f>
-        <v>47.199999999999996</v>
+        <v>49</v>
       </c>
       <c r="Q3">
         <f t="shared" ref="Q3:Q18" si="6">DEGREES(ATAN(($O$2-C3)/(2*A3*1.0647)))</f>
@@ -10312,8 +9615,7 @@
         <v>0.3</v>
       </c>
       <c r="B4">
-        <f>'X22 geometry data'!B45</f>
-        <v>50.199999999999996</v>
+        <v>46.8</v>
       </c>
       <c r="C4">
         <f>'X22 geometry data'!C45</f>
@@ -10324,7 +9626,7 @@
         <v>0.28439999999999999</v>
       </c>
       <c r="E4">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
@@ -10336,7 +9638,7 @@
       </c>
       <c r="I4">
         <f t="shared" si="2"/>
-        <v>44.899999999999991</v>
+        <v>45.8</v>
       </c>
       <c r="K4">
         <f t="shared" si="3"/>
@@ -10348,7 +9650,7 @@
       </c>
       <c r="M4">
         <f t="shared" si="5"/>
-        <v>44.899999999999991</v>
+        <v>45.8</v>
       </c>
       <c r="Q4">
         <f t="shared" si="6"/>
@@ -10361,8 +9663,7 @@
         <v>0.35</v>
       </c>
       <c r="B5">
-        <f>'X22 geometry data'!B46</f>
-        <v>48.8</v>
+        <v>43.2</v>
       </c>
       <c r="C5">
         <f>'X22 geometry data'!C46</f>
@@ -10385,7 +9686,7 @@
       </c>
       <c r="I5">
         <f t="shared" si="2"/>
-        <v>43.499999999999993</v>
+        <v>42.2</v>
       </c>
       <c r="K5">
         <f t="shared" si="3"/>
@@ -10397,7 +9698,7 @@
       </c>
       <c r="M5">
         <f t="shared" si="5"/>
-        <v>43.499999999999993</v>
+        <v>42.2</v>
       </c>
       <c r="Q5">
         <f t="shared" si="6"/>
@@ -10410,8 +9711,7 @@
         <v>0.4</v>
       </c>
       <c r="B6">
-        <f>'X22 geometry data'!B47</f>
-        <v>46.900000000000006</v>
+        <v>39.5</v>
       </c>
       <c r="C6">
         <f>'X22 geometry data'!C47</f>
@@ -10435,7 +9735,7 @@
       </c>
       <c r="I6">
         <f t="shared" si="2"/>
-        <v>41.6</v>
+        <v>38.5</v>
       </c>
       <c r="K6">
         <f t="shared" si="3"/>
@@ -10447,7 +9747,7 @@
       </c>
       <c r="M6">
         <f t="shared" si="5"/>
-        <v>41.6</v>
+        <v>38.5</v>
       </c>
       <c r="Q6">
         <f t="shared" si="6"/>
@@ -10460,8 +9760,7 @@
         <v>0.45</v>
       </c>
       <c r="B7">
-        <f>'X22 geometry data'!B48</f>
-        <v>45.199999999999996</v>
+        <v>35.9</v>
       </c>
       <c r="C7">
         <f>'X22 geometry data'!C48</f>
@@ -10481,7 +9780,7 @@
       </c>
       <c r="I7">
         <f t="shared" si="2"/>
-        <v>39.899999999999991</v>
+        <v>34.9</v>
       </c>
       <c r="K7">
         <f t="shared" si="3"/>
@@ -10493,7 +9792,7 @@
       </c>
       <c r="M7">
         <f t="shared" si="5"/>
-        <v>39.899999999999991</v>
+        <v>34.9</v>
       </c>
       <c r="Q7">
         <f t="shared" si="6"/>
@@ -10506,8 +9805,7 @@
         <v>0.5</v>
       </c>
       <c r="B8">
-        <f>'X22 geometry data'!B49</f>
-        <v>43.3</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="C8">
         <f>'X22 geometry data'!C49</f>
@@ -10530,7 +9828,7 @@
       </c>
       <c r="I8">
         <f t="shared" si="2"/>
-        <v>37.999999999999993</v>
+        <v>31.299999999999997</v>
       </c>
       <c r="K8">
         <f t="shared" si="3"/>
@@ -10542,7 +9840,7 @@
       </c>
       <c r="M8">
         <f t="shared" si="5"/>
-        <v>37.999999999999993</v>
+        <v>31.299999999999997</v>
       </c>
       <c r="Q8">
         <f t="shared" si="6"/>
@@ -10555,8 +9853,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="B9">
-        <f>'X22 geometry data'!B50</f>
-        <v>41.5</v>
+        <v>29.1</v>
       </c>
       <c r="C9">
         <f>'X22 geometry data'!C50</f>
@@ -10580,7 +9877,7 @@
       </c>
       <c r="I9">
         <f t="shared" si="2"/>
-        <v>36.199999999999996</v>
+        <v>28.1</v>
       </c>
       <c r="K9">
         <f t="shared" si="3"/>
@@ -10592,7 +9889,7 @@
       </c>
       <c r="M9">
         <f t="shared" si="5"/>
-        <v>36.199999999999996</v>
+        <v>28.1</v>
       </c>
       <c r="Q9">
         <f t="shared" si="6"/>
@@ -10605,8 +9902,7 @@
         <v>0.6</v>
       </c>
       <c r="B10">
-        <f>'X22 geometry data'!B51</f>
-        <v>39.6</v>
+        <v>26.4</v>
       </c>
       <c r="C10">
         <f>'X22 geometry data'!C51</f>
@@ -10626,7 +9922,7 @@
       </c>
       <c r="I10">
         <f t="shared" si="2"/>
-        <v>34.299999999999997</v>
+        <v>25.4</v>
       </c>
       <c r="K10">
         <f t="shared" si="3"/>
@@ -10638,7 +9934,7 @@
       </c>
       <c r="M10">
         <f t="shared" si="5"/>
-        <v>34.299999999999997</v>
+        <v>25.4</v>
       </c>
       <c r="Q10">
         <f t="shared" si="6"/>
@@ -10651,8 +9947,7 @@
         <v>0.65</v>
       </c>
       <c r="B11">
-        <f>'X22 geometry data'!B52</f>
-        <v>37.799999999999997</v>
+        <v>24.1</v>
       </c>
       <c r="C11">
         <f>'X22 geometry data'!C52</f>
@@ -10675,7 +9970,7 @@
       </c>
       <c r="I11">
         <f t="shared" si="2"/>
-        <v>32.499999999999993</v>
+        <v>23.1</v>
       </c>
       <c r="K11">
         <f t="shared" si="3"/>
@@ -10687,7 +9982,7 @@
       </c>
       <c r="M11">
         <f t="shared" si="5"/>
-        <v>32.499999999999993</v>
+        <v>23.1</v>
       </c>
       <c r="Q11">
         <f t="shared" si="6"/>
@@ -10700,8 +9995,7 @@
         <v>0.7</v>
       </c>
       <c r="B12">
-        <f>'X22 geometry data'!B53</f>
-        <v>35.9</v>
+        <v>21.8</v>
       </c>
       <c r="C12">
         <f>'X22 geometry data'!C53</f>
@@ -10725,7 +10019,7 @@
       </c>
       <c r="I12">
         <f t="shared" si="2"/>
-        <v>30.599999999999994</v>
+        <v>20.8</v>
       </c>
       <c r="K12">
         <f t="shared" si="3"/>
@@ -10737,7 +10031,7 @@
       </c>
       <c r="M12">
         <f t="shared" si="5"/>
-        <v>30.599999999999994</v>
+        <v>20.8</v>
       </c>
       <c r="Q12">
         <f t="shared" si="6"/>
@@ -10750,8 +10044,7 @@
         <v>0.75</v>
       </c>
       <c r="B13">
-        <f>'X22 geometry data'!B54</f>
-        <v>34.300000000000004</v>
+        <v>20</v>
       </c>
       <c r="C13">
         <f>'X22 geometry data'!C54</f>
@@ -10771,7 +10064,7 @@
       </c>
       <c r="I13">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="K13">
         <f t="shared" si="3"/>
@@ -10783,7 +10076,7 @@
       </c>
       <c r="M13">
         <f t="shared" si="5"/>
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="Q13">
         <f t="shared" si="6"/>
@@ -10796,8 +10089,7 @@
         <v>0.8</v>
       </c>
       <c r="B14">
-        <f>'X22 geometry data'!B55</f>
-        <v>32.5</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="C14">
         <f>'X22 geometry data'!C55</f>
@@ -10817,7 +10109,7 @@
       </c>
       <c r="I14">
         <f t="shared" si="2"/>
-        <v>27.199999999999996</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="K14">
         <f t="shared" si="3"/>
@@ -10829,7 +10121,7 @@
       </c>
       <c r="M14">
         <f t="shared" si="5"/>
-        <v>27.199999999999996</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="Q14">
         <f t="shared" si="6"/>
@@ -10842,8 +10134,7 @@
         <v>0.85</v>
       </c>
       <c r="B15">
-        <f>'X22 geometry data'!B56</f>
-        <v>30.8</v>
+        <v>17.7</v>
       </c>
       <c r="C15">
         <f>'X22 geometry data'!C56</f>
@@ -10863,7 +10154,7 @@
       </c>
       <c r="I15">
         <f t="shared" si="2"/>
-        <v>25.499999999999996</v>
+        <v>16.7</v>
       </c>
       <c r="K15">
         <f t="shared" si="3"/>
@@ -10875,7 +10166,7 @@
       </c>
       <c r="M15">
         <f t="shared" si="5"/>
-        <v>25.499999999999996</v>
+        <v>16.7</v>
       </c>
       <c r="Q15">
         <f t="shared" si="6"/>
@@ -10888,8 +10179,7 @@
         <v>0.9</v>
       </c>
       <c r="B16">
-        <f>'X22 geometry data'!B57</f>
-        <v>29</v>
+        <v>16.8</v>
       </c>
       <c r="C16">
         <f>'X22 geometry data'!C57</f>
@@ -10909,7 +10199,7 @@
       </c>
       <c r="I16">
         <f t="shared" si="2"/>
-        <v>23.699999999999996</v>
+        <v>15.8</v>
       </c>
       <c r="K16">
         <f t="shared" si="3"/>
@@ -10921,7 +10211,7 @@
       </c>
       <c r="M16">
         <f t="shared" si="5"/>
-        <v>23.699999999999996</v>
+        <v>15.8</v>
       </c>
       <c r="Q16">
         <f t="shared" si="6"/>
@@ -10934,8 +10224,7 @@
         <v>0.95</v>
       </c>
       <c r="B17">
-        <f>'X22 geometry data'!B58</f>
-        <v>27.9</v>
+        <v>15.9</v>
       </c>
       <c r="C17">
         <f>'X22 geometry data'!C58</f>
@@ -10955,7 +10244,7 @@
       </c>
       <c r="I17">
         <f t="shared" si="2"/>
-        <v>22.599999999999994</v>
+        <v>14.9</v>
       </c>
       <c r="K17">
         <f t="shared" si="3"/>
@@ -10967,7 +10256,7 @@
       </c>
       <c r="M17">
         <f t="shared" si="5"/>
-        <v>22.599999999999994</v>
+        <v>14.9</v>
       </c>
       <c r="Q17">
         <f t="shared" si="6"/>
@@ -10980,8 +10269,7 @@
         <v>1</v>
       </c>
       <c r="B18">
-        <f>'X22 geometry data'!B59</f>
-        <v>26.5</v>
+        <v>15.5</v>
       </c>
       <c r="C18">
         <f>'X22 geometry data'!C59</f>
@@ -11001,7 +10289,7 @@
       </c>
       <c r="I18">
         <f t="shared" si="2"/>
-        <v>21.199999999999996</v>
+        <v>14.5</v>
       </c>
       <c r="K18">
         <f t="shared" si="3"/>
@@ -11013,7 +10301,7 @@
       </c>
       <c r="M18">
         <f t="shared" si="5"/>
-        <v>21.199999999999996</v>
+        <v>14.5</v>
       </c>
       <c r="Q18">
         <f t="shared" si="6"/>
@@ -13698,12 +12986,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CF8B089-28A8-4FC7-8E68-349A1BA111DD}">
   <dimension ref="A2:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -14212,7 +13500,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{918BDE15-BB59-4315-AE6B-B1752C876129}">
   <dimension ref="A1:G92"/>
   <sheetViews>
@@ -16332,7 +15620,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92ADB1BB-9D21-4BA5-9552-1750A15434B2}">
   <dimension ref="A1:E35"/>
   <sheetViews>

</xml_diff>